<commit_message>
Update code as per the review points
</commit_message>
<xml_diff>
--- a/Ebay/Data.xlsx
+++ b/Ebay/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Login Page</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">SAMSUNG 65 INCHES 65MU6100 4K UHD LED TV 2017 MODEL + 1 YEAR DEALERS WARRANTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">₹120,000</t>
   </si>
   <si>
     <t xml:space="preserve">TV name and Discription on checkout page</t>
@@ -73,7 +76,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$₹-4009]#,##0.00;[RED]\-[$₹-4009]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -195,7 +198,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,17 +222,17 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.7044534412956"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -310,16 +313,16 @@
       <c r="A15" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="8" t="n">
-        <v>120000</v>
+      <c r="B15" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,7 +330,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>